<commit_message>
i have added add fuction
</commit_message>
<xml_diff>
--- a/exam.xlsx
+++ b/exam.xlsx
@@ -1,25 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Course\Data Analyst\Practice 2\collab2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A108DF03-62AB-4991-B923-66382C2A2BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +359,171 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D3:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>D4+E4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F15" si="0">D5+E5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>